<commit_message>
Fix: New name in config.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\Theresia\Fördelning av Lärarkostnad Per Gymnasiprogram\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\Theresia\RPA-Fordelning-Av-Lararkostnad-Per-Gymnasieprogram-Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -154,9 +154,6 @@
     <t>Exporter av lärarkostnader</t>
   </si>
   <si>
-    <t>Cred_APIGateway</t>
-  </si>
-  <si>
     <t>Cred_APIGatewayPerformer</t>
   </si>
   <si>
@@ -179,6 +176,9 @@
   </si>
   <si>
     <t>Skapa fasta fördelningar för gymnasielärare</t>
+  </si>
+  <si>
+    <t>Cred_APIGateway_Prod</t>
   </si>
 </sst>
 </file>
@@ -216,16 +216,16 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF464E55"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -247,7 +247,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -260,8 +260,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
@@ -580,7 +582,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -651,26 +653,26 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>43</v>
+      <c r="A6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1748,8 +1750,8 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>50</v>
+      <c r="B5" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -2891,13 +2893,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -2932,26 +2934,26 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added url in config.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450"/>
+    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -179,13 +179,16 @@
   </si>
   <si>
     <t>Cred_APIGateway_Prod</t>
+  </si>
+  <si>
+    <t>DomainURL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -227,6 +230,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF464E55"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -249,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -264,6 +273,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
@@ -581,7 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -2843,8 +2853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2956,7 +2966,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: Using dates from queueItem and added filepath to list for 'avvikande fördelning'. (not published)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>DomainURL</t>
+  </si>
+  <si>
+    <t>FilePathToFackligaRepresentanter</t>
+  </si>
+  <si>
+    <t>FilePathToAvvikandeFördelning</t>
   </si>
 </sst>
 </file>
@@ -2854,7 +2860,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A22" sqref="A22:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2974,7 +2980,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: Updated API, Heroma Web. not tested.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -188,13 +188,25 @@
   </si>
   <si>
     <t>FilePathToAvvikandeFördelning</t>
+  </si>
+  <si>
+    <t>URLBerit</t>
+  </si>
+  <si>
+    <t>Cred_NA_Berit</t>
+  </si>
+  <si>
+    <t>MunicipalityId</t>
+  </si>
+  <si>
+    <t>CitizensAPIVersion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -242,6 +254,18 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF464E55"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF464E55"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -264,7 +288,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -280,6 +304,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
@@ -595,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -691,8 +719,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9">
+        <v>2281</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1681,7 +1723,6 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2860,7 +2901,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:B29"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2988,8 +3029,22 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>